<commit_message>
Check effect of interest rate on optimal solution
</commit_message>
<xml_diff>
--- a/model/model_inputs_feedin.xlsx
+++ b/model/model_inputs_feedin.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{23151FC7-BF80-49E4-993D-8B11E77D56F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F42FBF3-11AF-4569-865E-FE1421CC2EEC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2501,7 +2501,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2563,10 +2563,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>20</v>
@@ -2586,10 +2586,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
@@ -3750,14 +3750,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D835CF4C7D56B243BA013D4D2E10914B" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e645ef68b9493f2ee8bae9e534bc24f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6d4e152b-60f6-4719-8921-68b5b8011cde" xmlns:ns4="28683373-984a-4841-9f0e-018f3f7bab1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a06da6e71fc3d3bdf7cbe176c2a8afa1" ns3:_="" ns4:_="">
     <xsd:import namespace="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
@@ -4010,6 +4002,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
   <ds:schemaRefs>
@@ -4019,23 +4019,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
-    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCE4FBA5-6C26-4B97-9218-92B658F853C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4052,4 +4035,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
+    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add unmet demand model folder
</commit_message>
<xml_diff>
--- a/model/model_inputs_feedin.xlsx
+++ b/model/model_inputs_feedin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{768A0861-2BF3-4683-9E1A-8EB23133B487}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BE26905-3926-4E1F-A997-66DCA5D7959B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,17 @@
     <sheet name="tech" sheetId="6" r:id="rId3"/>
     <sheet name="tariffs" sheetId="7" r:id="rId4"/>
     <sheet name="heat_rate" sheetId="8" r:id="rId5"/>
-    <sheet name="capacity_steps" sheetId="13" r:id="rId6"/>
-    <sheet name="day_weights" sheetId="2" r:id="rId7"/>
-    <sheet name="cap_factors" sheetId="4" r:id="rId8"/>
-    <sheet name="elec_demand (1)" sheetId="3" r:id="rId9"/>
-    <sheet name="elec_demand (2)" sheetId="9" r:id="rId10"/>
-    <sheet name="elec_demand (3)" sheetId="10" r:id="rId11"/>
-    <sheet name="elec_demand (4)" sheetId="11" r:id="rId12"/>
-    <sheet name="elec_demand (5)" sheetId="12" r:id="rId13"/>
+    <sheet name="day_weights" sheetId="2" r:id="rId6"/>
+    <sheet name="cap_factors" sheetId="4" r:id="rId7"/>
+    <sheet name="elec_demand (1)" sheetId="3" r:id="rId8"/>
+    <sheet name="elec_demand (2)" sheetId="9" r:id="rId9"/>
+    <sheet name="elec_demand (3)" sheetId="10" r:id="rId10"/>
+    <sheet name="elec_demand (4)" sheetId="11" r:id="rId11"/>
+    <sheet name="elec_demand (5)" sheetId="12" r:id="rId12"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId14"/>
-  </externalReferences>
+  <definedNames>
+    <definedName name="d">'elec_demand (2)'!$B$6:$Y$8</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>min SoC</t>
   </si>
@@ -108,9 +107,6 @@
     <t>Diesel Price</t>
   </si>
   <si>
-    <t>Ministry Tariff</t>
-  </si>
-  <si>
     <t>year 1</t>
   </si>
   <si>
@@ -189,7 +185,16 @@
     <t>60%-100%</t>
   </si>
   <si>
-    <t>Avg PV capacity (Wp)</t>
+    <t>summer</t>
+  </si>
+  <si>
+    <t>fall_spring</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>Avg PV capacity (kWp)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +204,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +217,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -228,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -236,11 +246,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -254,6 +279,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,84 +298,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Techs"/>
-      <sheetName val="Sources"/>
-      <sheetName val="Capacity Factors"/>
-      <sheetName val="LCOE of PV and DG"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="C2">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>84.069000000000003</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>1.4000710227272728E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>975</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>21.8</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>1.38E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>352</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>60.8</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>0.6</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -668,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,449 +677,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867F374D-6AFF-43B6-B370-B2ECC1DAC459}">
-  <dimension ref="A1:Y31"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="25" width="6.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="M1">
-        <v>11</v>
-      </c>
-      <c r="N1">
-        <v>12</v>
-      </c>
-      <c r="O1">
-        <v>13</v>
-      </c>
-      <c r="P1">
-        <v>14</v>
-      </c>
-      <c r="Q1">
-        <v>15</v>
-      </c>
-      <c r="R1">
-        <v>16</v>
-      </c>
-      <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
-        <v>18</v>
-      </c>
-      <c r="U1">
-        <v>19</v>
-      </c>
-      <c r="V1">
-        <v>20</v>
-      </c>
-      <c r="W1">
-        <v>21</v>
-      </c>
-      <c r="X1">
-        <v>22</v>
-      </c>
-      <c r="Y1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.78900000000000003</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.70399999999999996</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.79800000000000004</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.7410000000000001</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.70500000000000007</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0.71000000000000008</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0.69400000000000006</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0.78400000000000003</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0.88</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0.71399999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.42</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="R3" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="S3" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="T3" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="U3" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="V3" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="W3" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="X3" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.74500000000000011</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.622</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.60699999999999998</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.81099999999999994</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0.76300000000000001</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0.73799999999999999</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0.74</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0.746</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="T4" s="6">
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0.93399999999999994</v>
-      </c>
-      <c r="W4" s="6">
-        <v>0.93499999999999994</v>
-      </c>
-      <c r="X4" s="6">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="Y4" s="6">
-        <v>0.83799999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01985ED-3AF2-4182-BB5C-CF8628DEF823}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -1257,7 +765,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5">
         <v>0.50900000000000001</v>
@@ -1334,7 +842,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6">
         <v>0.27</v>
@@ -1411,7 +919,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6">
         <v>0.46500000000000002</v>
@@ -1611,7 +1119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F25FDCC-0E53-468A-95CC-401F964650F2}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -1700,7 +1208,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -1777,7 +1285,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -1854,7 +1362,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5">
         <v>0</v>
@@ -2054,7 +1562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE540155-C042-4D87-9ACA-1F490BE78401}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -2143,7 +1651,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5">
         <v>0.5</v>
@@ -2220,7 +1728,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6">
         <v>0.5</v>
@@ -2297,7 +1805,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6">
         <v>0.5</v>
@@ -2502,12 +2010,12 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6328125" customWidth="1"/>
@@ -2537,10 +2045,10 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>840</v>
+        <v>265</v>
       </c>
       <c r="C2">
-        <v>510</v>
+        <v>184</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -2554,13 +2062,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2581,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C15:C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2627,18 +2135,15 @@
         <v>3</v>
       </c>
       <c r="D2" s="6">
-        <f>[1]Sources!C2</f>
         <v>5</v>
       </c>
       <c r="E2">
-        <v>180</v>
+        <v>800</v>
       </c>
       <c r="F2" s="6">
-        <f>[1]Sources!C5</f>
         <v>84.069000000000003</v>
       </c>
       <c r="G2">
-        <f>[1]Sources!C6</f>
         <v>1.4000710227272728E-2</v>
       </c>
     </row>
@@ -2653,19 +2158,15 @@
         <v>0</v>
       </c>
       <c r="D3" s="6">
-        <f>[1]Sources!C7</f>
         <v>25</v>
       </c>
       <c r="E3" s="6">
-        <f>[1]Sources!C8</f>
         <v>975</v>
       </c>
       <c r="F3" s="6">
-        <f>[1]Sources!C9</f>
         <v>21.8</v>
       </c>
       <c r="G3">
-        <f>[1]Sources!C10</f>
         <v>1.38E-2</v>
       </c>
     </row>
@@ -2680,19 +2181,15 @@
         <v>0</v>
       </c>
       <c r="D4" s="6">
-        <f>[1]Sources!C11</f>
         <v>12</v>
       </c>
       <c r="E4" s="6">
-        <f>[1]Sources!C13</f>
         <v>352</v>
       </c>
       <c r="F4" s="6">
-        <f>[1]Sources!C14</f>
         <v>60.8</v>
       </c>
       <c r="G4" s="6">
-        <f>[1]Sources!C15</f>
         <v>0.6</v>
       </c>
     </row>
@@ -2703,190 +2200,141 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45D110-F0D2-4F9D-B0C4-13B38005F879}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>23</v>
       </c>
       <c r="B2">
         <v>0.80323299888517286</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0.7998018797075267</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>0.79636610600256064</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>0.79292564496168683</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.78948046335616628</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.13500000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>0.78603052752928926</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.13900000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>0.78257580338835164</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>0.77911625639644011</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.14699999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>0.77565185156400585</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>0.77218255344024267</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>0.76870832610423512</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>0.76522913315588315</v>
       </c>
-      <c r="C13" s="1">
-        <v>0.16300000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>0.76174493770661011</v>
       </c>
-      <c r="C14" s="1">
-        <v>0.16700000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>0.75825570236981887</v>
       </c>
-      <c r="C15" s="1">
-        <v>0.17100000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>0.75476138925110314</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.17499999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2913,12 +2361,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <f>(-0.2129*(0.3^3+0^3) +0.6056*(0.3^2+0^2) - 0.5538*(0.3+0) + 0.4067*2)/2</f>
@@ -2930,7 +2378,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <f>(-0.2129*(0.6^3+0.3^3) +0.6056*(0.6^2+0.3^2) - 0.5538*(0.6+0.3) + 0.4067*2)/2</f>
@@ -2942,7 +2390,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <f>(-0.2129*(1^3+0.6^3) +0.6056*(1^2+0.6^2) - 0.5538*(1+0.6) + 0.4067*2)/2</f>
@@ -2958,85 +2406,366 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDB5C9E-DDE6-4406-A1BA-E0B87BADDE72}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB9A018-F4D8-4049-8785-D914448B1EBA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="8">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>198</v>
+        <v>40</v>
+      </c>
+      <c r="B3" s="8">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="B4" s="8">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
+  <dimension ref="A1:Y4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="5.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2.5819672131147539E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.16275409836065571</v>
+      </c>
+      <c r="J2">
+        <v>0.37470491803278688</v>
+      </c>
+      <c r="K2">
+        <v>0.5609016393442624</v>
+      </c>
+      <c r="L2">
+        <v>0.69518032786885242</v>
+      </c>
+      <c r="M2">
+        <v>0.77686065573770491</v>
+      </c>
+      <c r="N2">
+        <v>0.81105737704918035</v>
+      </c>
+      <c r="O2">
+        <v>0.7935245901639344</v>
+      </c>
+      <c r="P2">
+        <v>0.72468852459016386</v>
+      </c>
+      <c r="Q2">
+        <v>0.60230327868852451</v>
+      </c>
+      <c r="R2">
+        <v>0.43349180327868853</v>
+      </c>
+      <c r="S2">
+        <v>0.23055737704918031</v>
+      </c>
+      <c r="T2">
+        <v>5.0016393442622951E-2</v>
+      </c>
+      <c r="U2">
+        <v>2.991803278688524E-3</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1.335294117647059E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.1510457516339869</v>
+      </c>
+      <c r="J3">
+        <v>0.36648366013071898</v>
+      </c>
+      <c r="K3">
+        <v>0.54676470588235293</v>
+      </c>
+      <c r="L3">
+        <v>0.66818954248366014</v>
+      </c>
+      <c r="M3">
+        <v>0.73162745098039206</v>
+      </c>
+      <c r="N3">
+        <v>0.74206535947712415</v>
+      </c>
+      <c r="O3">
+        <v>0.70073202614379082</v>
+      </c>
+      <c r="P3">
+        <v>0.59535947712418302</v>
+      </c>
+      <c r="Q3">
+        <v>0.43600653594771238</v>
+      </c>
+      <c r="R3">
+        <v>0.24354901960784309</v>
+      </c>
+      <c r="S3">
+        <v>0.11178431372549021</v>
+      </c>
+      <c r="T3">
+        <v>1.822875816993464E-2</v>
+      </c>
+      <c r="U3">
+        <v>4.3790849673202621E-4</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>106</v>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4.3956043956043948E-5</v>
+      </c>
+      <c r="H4">
+        <v>3.9714285714285723E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.1988681318681319</v>
+      </c>
+      <c r="J4">
+        <v>0.3788791208791209</v>
+      </c>
+      <c r="K4">
+        <v>0.52748351648351643</v>
+      </c>
+      <c r="L4">
+        <v>0.62382417582417582</v>
+      </c>
+      <c r="M4">
+        <v>0.66321978021978023</v>
+      </c>
+      <c r="N4">
+        <v>0.6375384615384615</v>
+      </c>
+      <c r="O4">
+        <v>0.55946153846153845</v>
+      </c>
+      <c r="P4">
+        <v>0.43716483516483517</v>
+      </c>
+      <c r="Q4">
+        <v>0.26671428571428568</v>
+      </c>
+      <c r="R4">
+        <v>8.4153846153846162E-2</v>
+      </c>
+      <c r="S4">
+        <v>4.6263736263736262E-3</v>
+      </c>
+      <c r="T4">
+        <v>2.5274725274725281E-4</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3045,335 +2774,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
-  <dimension ref="A1:Y4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="5.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1.8032786885245899E-3</v>
-      </c>
-      <c r="H2">
-        <v>1.6032786885245912E-2</v>
-      </c>
-      <c r="I2">
-        <v>5.4229508196721322E-2</v>
-      </c>
-      <c r="J2">
-        <v>0.1274918032786885</v>
-      </c>
-      <c r="K2">
-        <v>0.20950819672131141</v>
-      </c>
-      <c r="L2">
-        <v>0.26809836065573772</v>
-      </c>
-      <c r="M2">
-        <v>0.28267213114754092</v>
-      </c>
-      <c r="N2">
-        <v>0.27595081967213131</v>
-      </c>
-      <c r="O2">
-        <v>0.25488524590163941</v>
-      </c>
-      <c r="P2">
-        <v>0.21809836065573759</v>
-      </c>
-      <c r="Q2">
-        <v>0.151</v>
-      </c>
-      <c r="R2">
-        <v>8.1081967213114725E-2</v>
-      </c>
-      <c r="S2">
-        <v>3.1426229508196707E-2</v>
-      </c>
-      <c r="T2">
-        <v>7.7049180327868824E-3</v>
-      </c>
-      <c r="U2">
-        <v>9.8360655737705021E-5</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>4.0201005025125598E-3</v>
-      </c>
-      <c r="H3">
-        <v>4.1170854271356763E-2</v>
-      </c>
-      <c r="I3">
-        <v>0.15498492462311561</v>
-      </c>
-      <c r="J3">
-        <v>0.34120100502512568</v>
-      </c>
-      <c r="K3">
-        <v>0.51137185929648243</v>
-      </c>
-      <c r="L3">
-        <v>0.63440201005025132</v>
-      </c>
-      <c r="M3">
-        <v>0.70589447236180902</v>
-      </c>
-      <c r="N3">
-        <v>0.7173165829145729</v>
-      </c>
-      <c r="O3">
-        <v>0.67734170854271358</v>
-      </c>
-      <c r="P3">
-        <v>0.57809547738693468</v>
-      </c>
-      <c r="Q3">
-        <v>0.43412562814070349</v>
-      </c>
-      <c r="R3">
-        <v>0.25252763819095481</v>
-      </c>
-      <c r="S3">
-        <v>9.1608040201005048E-2</v>
-      </c>
-      <c r="T3">
-        <v>1.7597989949748739E-2</v>
-      </c>
-      <c r="U3">
-        <v>3.2160804020100472E-4</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>2.1509433962264152E-3</v>
-      </c>
-      <c r="H4">
-        <v>2.0773584905660381E-2</v>
-      </c>
-      <c r="I4">
-        <v>7.4056603773584917E-2</v>
-      </c>
-      <c r="J4">
-        <v>0.20321698113207551</v>
-      </c>
-      <c r="K4">
-        <v>0.34733018867924531</v>
-      </c>
-      <c r="L4">
-        <v>0.46702830188679251</v>
-      </c>
-      <c r="M4">
-        <v>0.54499999999999993</v>
-      </c>
-      <c r="N4">
-        <v>0.55942452830188683</v>
-      </c>
-      <c r="O4">
-        <v>0.51176415094339622</v>
-      </c>
-      <c r="P4">
-        <v>0.41073584905660382</v>
-      </c>
-      <c r="Q4">
-        <v>0.27456603773584909</v>
-      </c>
-      <c r="R4">
-        <v>0.13354716981132081</v>
-      </c>
-      <c r="S4">
-        <v>3.995283018867922E-2</v>
-      </c>
-      <c r="T4">
-        <v>8.6698113207547139E-3</v>
-      </c>
-      <c r="U4">
-        <v>1.4150943396226421E-4</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABED9F3-A079-4BB6-8141-C898B88CBE8C}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:Y7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3457,7 +2862,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5">
         <v>0.93899999999999995</v>
@@ -3534,7 +2939,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6">
         <v>0.7</v>
@@ -3611,7 +3016,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6">
         <v>0.89500000000000002</v>
@@ -3731,6 +3136,429 @@
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867F374D-6AFF-43B6-B370-B2ECC1DAC459}">
+  <dimension ref="A1:Y31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="25" width="6.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.3415913978494623</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.3032688172043011</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.29459139784946226</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.28721505376344075</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.29210752688172037</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.29610752688172037</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.31112903225806449</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.345741935483871</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.38683870967741929</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.41622580645161295</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.45535483870967736</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.41387096774193538</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0.37684946236559141</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0.3618279569892473</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0.33379569892473121</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0.3368387096774193</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0.3406989247311828</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0.3688709677419354</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0.40449462365591399</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0.4571935483870968</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0.47998924731182802</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0.46408602150537631</v>
+      </c>
+      <c r="X2" s="6">
+        <v>0.4129677419354838</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>0.40031182795698916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5">
+        <v>9.8233310344827587E-2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.10124206896551721</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.1033535632183908</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.101562816091954</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.10336005747126439</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.1031586206896552</v>
+      </c>
+      <c r="H3" s="6">
+        <v>9.2196494252873559E-2</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.16613097701149432</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.20496649425287358</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.148505517241379</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.14703405596382191</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.23111904371584641</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.107144367816092</v>
+      </c>
+      <c r="O3" s="6">
+        <v>9.9946598831727445E-3</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0.4522793631053329</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>6.4428272093461372E-2</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0.52805508856227656</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0.54662643935159305</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0.25055333333333329</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0.20713979444444439</v>
+      </c>
+      <c r="V3" s="6">
+        <v>0.18756173888888888</v>
+      </c>
+      <c r="W3" s="6">
+        <v>0.18910446111111109</v>
+      </c>
+      <c r="X3" s="6">
+        <v>0.1889352222222222</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>0.18806571666666658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5">
+        <v>9.8233310344827587E-2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.10124206896551721</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.1033535632183908</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.101562816091954</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.10336005747126439</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.1031586206896552</v>
+      </c>
+      <c r="H4" s="6">
+        <v>9.2196494252873559E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.16613097701149432</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.20496649425287358</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1.0175055172413789</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1.5168291379310348</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1.802061666666666</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1.8921443678160921</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1.992822528735632</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1.955951494252874</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1.781165977011494</v>
+      </c>
+      <c r="R4" s="6">
+        <v>1.485719022988506</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0.54662643935159305</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0.25055333333333329</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0.20713979444444439</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0.18756173888888888</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0.18910446111111109</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0.1889352222222222</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0.18806571666666658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>

</xml_diff>

<commit_message>
Update inputs, obtain trial outputs
</commit_message>
<xml_diff>
--- a/model/model_inputs_feedin.xlsx
+++ b/model/model_inputs_feedin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BE26905-3926-4E1F-A997-66DCA5D7959B}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB83D6F9-86C7-443A-8984-824825FB730C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
     <sheet name="cap_factors" sheetId="4" r:id="rId7"/>
     <sheet name="elec_demand (1)" sheetId="3" r:id="rId8"/>
     <sheet name="elec_demand (2)" sheetId="9" r:id="rId9"/>
-    <sheet name="elec_demand (3)" sheetId="10" r:id="rId10"/>
-    <sheet name="elec_demand (4)" sheetId="11" r:id="rId11"/>
-    <sheet name="elec_demand (5)" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="d">'elec_demand (2)'!$B$6:$Y$8</definedName>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>min SoC</t>
   </si>
@@ -63,15 +60,6 @@
   </si>
   <si>
     <t>Type 2</t>
-  </si>
-  <si>
-    <t>Type 3</t>
-  </si>
-  <si>
-    <t>Type 4</t>
-  </si>
-  <si>
-    <t>Type 5</t>
   </si>
   <si>
     <t>No available</t>
@@ -222,6 +210,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -265,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -282,7 +271,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -676,1341 +664,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01985ED-3AF2-4182-BB5C-CF8628DEF823}">
-  <dimension ref="A1:Y31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="25" width="6.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="M1">
-        <v>11</v>
-      </c>
-      <c r="N1">
-        <v>12</v>
-      </c>
-      <c r="O1">
-        <v>13</v>
-      </c>
-      <c r="P1">
-        <v>14</v>
-      </c>
-      <c r="Q1">
-        <v>15</v>
-      </c>
-      <c r="R1">
-        <v>16</v>
-      </c>
-      <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
-        <v>18</v>
-      </c>
-      <c r="U1">
-        <v>19</v>
-      </c>
-      <c r="V1">
-        <v>20</v>
-      </c>
-      <c r="W1">
-        <v>21</v>
-      </c>
-      <c r="X1">
-        <v>22</v>
-      </c>
-      <c r="Y1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.50900000000000001</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.47299999999999998</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.46699999999999997</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.51100000000000001</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.59800000000000009</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.59099999999999997</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.57000000000000006</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0.51</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0.504</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0.44899999999999995</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0.50900000000000001</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0.53400000000000003</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0.54099999999999993</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0.41399999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.27</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="R3" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="S3" s="6">
-        <v>0.37</v>
-      </c>
-      <c r="T3" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="U3" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="V3" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="W3" s="6">
-        <v>0.42</v>
-      </c>
-      <c r="X3" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.45399999999999996</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.65900000000000003</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0.57199999999999995</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0.52600000000000002</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="T4" s="6">
-        <v>0.63100000000000001</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0.68200000000000005</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="W4" s="6">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="X4" s="6">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="Y4" s="6">
-        <v>0.53800000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F25FDCC-0E53-468A-95CC-401F964650F2}">
-  <dimension ref="A1:Y31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="25" width="6.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>35</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>35</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>35</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>35</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <v>0</v>
-      </c>
-      <c r="W3" s="5">
-        <v>0</v>
-      </c>
-      <c r="X3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>35</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5">
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>35</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
-        <v>0</v>
-      </c>
-      <c r="W4" s="5">
-        <v>0</v>
-      </c>
-      <c r="X4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE540155-C042-4D87-9ACA-1F490BE78401}">
-  <dimension ref="A1:Y31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:Y7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="25" width="6.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="I2" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="J2" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K2" s="5">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="N2" s="5">
-        <v>1</v>
-      </c>
-      <c r="O2" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="P2" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>1</v>
-      </c>
-      <c r="R2" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="S2" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="T2" s="5">
-        <v>2</v>
-      </c>
-      <c r="U2" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="V2" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="W2" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="N3" s="6">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>1</v>
-      </c>
-      <c r="R3" s="6">
-        <v>0</v>
-      </c>
-      <c r="S3" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="T3" s="6">
-        <v>2</v>
-      </c>
-      <c r="U3" s="6">
-        <v>0</v>
-      </c>
-      <c r="V3" s="6">
-        <v>0</v>
-      </c>
-      <c r="W3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="X3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6">
-        <v>2</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0</v>
-      </c>
-      <c r="W4" s="6">
-        <v>0</v>
-      </c>
-      <c r="X4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E688FB98-37F3-4971-B4CD-1E6A7262204F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2018,66 +677,36 @@
     <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.08984375" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2">
-        <v>265</v>
+        <v>635</v>
       </c>
       <c r="C2">
-        <v>184</v>
-      </c>
-      <c r="D2">
-        <v>40</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
         <v>4</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>123</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2106,27 +735,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>400</v>
@@ -2149,7 +778,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2172,7 +801,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2214,12 +843,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>0.80323299888517286</v>
@@ -2227,7 +856,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0.7998018797075267</v>
@@ -2235,7 +864,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>0.79636610600256064</v>
@@ -2243,7 +872,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0.79292564496168683</v>
@@ -2251,7 +880,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>0.78948046335616628</v>
@@ -2259,7 +888,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>0.78603052752928926</v>
@@ -2267,7 +896,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>0.78257580338835164</v>
@@ -2275,7 +904,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0.77911625639644011</v>
@@ -2283,7 +912,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>0.77565185156400585</v>
@@ -2291,7 +920,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>0.77218255344024267</v>
@@ -2299,7 +928,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>0.76870832610423512</v>
@@ -2307,7 +936,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>0.76522913315588315</v>
@@ -2315,7 +944,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>0.76174493770661011</v>
@@ -2323,7 +952,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>0.75825570236981887</v>
@@ -2331,7 +960,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>0.75476138925110314</v>
@@ -2361,12 +990,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <f>(-0.2129*(0.3^3+0^3) +0.6056*(0.3^2+0^2) - 0.5538*(0.3+0) + 0.4067*2)/2</f>
@@ -2378,7 +1007,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <f>(-0.2129*(0.6^3+0.3^3) +0.6056*(0.6^2+0.3^2) - 0.5538*(0.6+0.3) + 0.4067*2)/2</f>
@@ -2390,7 +1019,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <f>(-0.2129*(1^3+0.6^3) +0.6056*(1^2+0.6^2) - 0.5538*(1+0.6) + 0.4067*2)/2</f>
@@ -2417,30 +1046,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="8">
+        <v>36</v>
+      </c>
+      <c r="B2">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="8">
+        <v>37</v>
+      </c>
+      <c r="B3">
         <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="8">
+        <v>38</v>
+      </c>
+      <c r="B4">
         <v>121</v>
       </c>
     </row>
@@ -2539,7 +1168,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2616,7 +1245,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2693,7 +1322,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2862,7 +1491,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5">
         <v>0.93899999999999995</v>
@@ -2939,7 +1568,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="6">
         <v>0.7</v>
@@ -3016,7 +1645,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6">
         <v>0.89500000000000002</v>
@@ -3242,7 +1871,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3326,233 +1955,233 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5">
-        <v>0.3415913978494623</v>
+        <v>0.52236078409734032</v>
       </c>
       <c r="C2" s="5">
-        <v>0.3032688172043011</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.29459139784946226</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.28721505376344075</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.29210752688172037</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.29610752688172037</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0.31112903225806449</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0.345741935483871</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0.38683870967741929</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0.41622580645161295</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0.45535483870967736</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0.41387096774193538</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0.37684946236559141</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0.3618279569892473</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0.33379569892473121</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0.3368387096774193</v>
-      </c>
-      <c r="R2" s="6">
-        <v>0.3406989247311828</v>
-      </c>
-      <c r="S2" s="6">
-        <v>0.3688709677419354</v>
-      </c>
-      <c r="T2" s="6">
-        <v>0.40449462365591399</v>
-      </c>
-      <c r="U2" s="6">
-        <v>0.4571935483870968</v>
-      </c>
-      <c r="V2" s="6">
-        <v>0.47998924731182802</v>
-      </c>
-      <c r="W2" s="6">
-        <v>0.46408602150537631</v>
-      </c>
-      <c r="X2" s="6">
-        <v>0.4129677419354838</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>0.40031182795698916</v>
+        <v>0.4976949585403172</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.44207707194659279</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.43777742669441688</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.43521624705520451</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.44168559400742047</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.43422701750307208</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0.57877143627095295</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.49813638937877719</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0.36220495359399552</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0.63254991786411985</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0.76515335565616571</v>
+      </c>
+      <c r="T2" s="5">
+        <v>0.69171444098597745</v>
+      </c>
+      <c r="U2" s="5">
+        <v>0.70649159906935721</v>
+      </c>
+      <c r="V2" s="5">
+        <v>0.65930040212538521</v>
+      </c>
+      <c r="W2" s="5">
+        <v>0.68374114412375109</v>
+      </c>
+      <c r="X2" s="5">
+        <v>0.6465764204867005</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>0.52784287934130891</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5">
-        <v>9.8233310344827587E-2</v>
+        <v>0.4532206627457997</v>
       </c>
       <c r="C3" s="5">
-        <v>0.10124206896551721</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0.1033535632183908</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.101562816091954</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.10336005747126439</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.1031586206896552</v>
-      </c>
-      <c r="H3" s="6">
-        <v>9.2196494252873559E-2</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.16613097701149432</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0.20496649425287358</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0.148505517241379</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.14703405596382191</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.23111904371584641</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0.107144367816092</v>
-      </c>
-      <c r="O3" s="6">
-        <v>9.9946598831727445E-3</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0.4522793631053329</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>6.4428272093461372E-2</v>
-      </c>
-      <c r="R3" s="6">
-        <v>0.52805508856227656</v>
-      </c>
-      <c r="S3" s="6">
-        <v>0.54662643935159305</v>
-      </c>
-      <c r="T3" s="6">
-        <v>0.25055333333333329</v>
-      </c>
-      <c r="U3" s="6">
-        <v>0.20713979444444439</v>
-      </c>
-      <c r="V3" s="6">
-        <v>0.18756173888888888</v>
-      </c>
-      <c r="W3" s="6">
-        <v>0.18910446111111109</v>
-      </c>
-      <c r="X3" s="6">
-        <v>0.1889352222222222</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>0.18806571666666658</v>
+        <v>0.42851577557190434</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.41006267002011798</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.40494640291925321</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.39784783272475621</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.38054976568865906</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.355582734009113</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.28022226441607873</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.26214099497469462</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.26214099497469462</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.26214099497469462</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.37042423631317345</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.33010671286708548</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.26214099497469462</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0.26214099497469462</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0.26214099497469462</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.39731347710975679</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0.46361519600577983</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.4268957386706857</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0.43428431771237552</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0.42149519720844475</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0.4546003728097659</v>
+      </c>
+      <c r="X3" s="5">
+        <v>0.45266785406408228</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0.42511548495894508</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5">
-        <v>9.8233310344827587E-2</v>
+        <v>0.38408054139425912</v>
       </c>
       <c r="C4" s="5">
-        <v>0.10124206896551721</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.1033535632183908</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.101562816091954</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.10336005747126439</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.1031586206896552</v>
-      </c>
-      <c r="H4" s="6">
-        <v>9.2196494252873559E-2</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.16613097701149432</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0.20496649425287358</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1.0175055172413789</v>
-      </c>
-      <c r="L4" s="6">
-        <v>1.5168291379310348</v>
-      </c>
-      <c r="M4" s="6">
-        <v>1.802061666666666</v>
-      </c>
-      <c r="N4" s="6">
-        <v>1.8921443678160921</v>
-      </c>
-      <c r="O4" s="6">
-        <v>1.992822528735632</v>
-      </c>
-      <c r="P4" s="6">
-        <v>1.955951494252874</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>1.781165977011494</v>
-      </c>
-      <c r="R4" s="6">
-        <v>1.485719022988506</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0.54662643935159305</v>
-      </c>
-      <c r="T4" s="6">
-        <v>0.25055333333333329</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0.20713979444444439</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0.18756173888888888</v>
-      </c>
-      <c r="W4" s="6">
-        <v>0.18910446111111109</v>
-      </c>
-      <c r="X4" s="6">
-        <v>0.1889352222222222</v>
-      </c>
-      <c r="Y4" s="6">
-        <v>0.18806571666666658</v>
+        <v>0.35933659260349149</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.37804826809364339</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.37211537914408938</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.36047941839430803</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.3194139373698977</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.27693845051515387</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.19823957523816191</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0.16207703635539389</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0.1836899922915041</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0.22545960149578079</v>
+      </c>
+      <c r="X4" s="5">
+        <v>0.25875928764146422</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0.32238809057658119</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">

</xml_diff>